<commit_message>
820960 100218 updates to address review findings
</commit_message>
<xml_diff>
--- a/Test/Build 4/TAS eBill TEL IB_2.0_592.xlsx
+++ b/Test/Build 4/TAS eBill TEL IB_2.0_592.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="4812" windowWidth="23016" windowHeight="5436" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="4812" windowWidth="23016" windowHeight="5436" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="137">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -430,8 +430,47 @@
     <t>September 2018</t>
   </si>
   <si>
+    <t>Updated with test results for final build T20 testing.</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T20</t>
+  </si>
+  <si>
+    <t>TC1370 - CIT  eBilling Create an Outpatient  Claim via Autobiller - Regression  US1109</t>
+  </si>
+  <si>
+    <t>TC1370 - CIT  eBilling Create an Outpatient  Claim via Autobiller - Regression US1109</t>
+  </si>
+  <si>
+    <t>DE832</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T15</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T17</t>
+  </si>
+  <si>
+    <t>DE894</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T18</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T19</t>
+  </si>
+  <si>
+    <t>DE893</t>
+  </si>
+  <si>
+    <t>DE845</t>
+  </si>
+  <si>
+    <t>October 2018</t>
+  </si>
+  <si>
     <r>
-      <t>Version 4.0</t>
+      <t>Version 5.0</t>
     </r>
     <r>
       <rPr>
@@ -445,43 +484,16 @@
     </r>
   </si>
   <si>
-    <t>Updated with test results for final build T20 testing.</t>
-  </si>
-  <si>
-    <t>IB*2.0*592_T20</t>
-  </si>
-  <si>
-    <t>TC1370 - CIT  eBilling Create an Outpatient  Claim via Autobiller - Regression  US1109</t>
-  </si>
-  <si>
-    <t>TC1370 - CIT  eBilling Create an Outpatient  Claim via Autobiller - Regression US1109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC2231 - CIT eBilling US2488 - Update Reports - Form Type J430D - Regression </t>
-  </si>
-  <si>
-    <t>DE832</t>
-  </si>
-  <si>
-    <t>IB*2.0*592_T15</t>
-  </si>
-  <si>
-    <t>IB*2.0*592_T17</t>
-  </si>
-  <si>
-    <t>DE894</t>
-  </si>
-  <si>
-    <t>IB*2.0*592_T18</t>
-  </si>
-  <si>
-    <t>IB*2.0*592_T19</t>
-  </si>
-  <si>
-    <t>DE893</t>
-  </si>
-  <si>
-    <t>DE845</t>
+    <t xml:space="preserve">TC2534 - CIT eBilling TS27 – Dental Claim Creation – AutoBiller- Auto Populated Fields – Production Only </t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T11</t>
+  </si>
+  <si>
+    <t>TC2231 - CIT eBilling US2488 - Update Reports - Form Type J430D - Regression Not aaplicable</t>
+  </si>
+  <si>
+    <t>Updated to add TC2534, which was added in Feb, and so that it may coincide with the TEL</t>
   </si>
 </sst>
 </file>
@@ -2300,7 +2312,7 @@
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="100" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B26" s="100"/>
       <c r="C26" s="100"/>
@@ -2349,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2437,17 +2449,25 @@
         <v>4</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="55"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="66"/>
+    <row r="8" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="65">
+        <v>5</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="72"/>
@@ -2493,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX312"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J214" sqref="J214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2604,7 +2624,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="46">
         <v>43361</v>
@@ -2698,7 +2718,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="46">
         <v>43360</v>
@@ -2792,7 +2812,7 @@
         <v>37</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" s="46">
         <v>42996</v>
@@ -2886,7 +2906,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16" s="46">
         <v>43360</v>
@@ -2980,7 +3000,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="46">
         <v>43361</v>
@@ -3074,7 +3094,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="46">
         <v>43361</v>
@@ -3168,7 +3188,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" s="46">
         <v>43361</v>
@@ -3262,7 +3282,7 @@
         <v>37</v>
       </c>
       <c r="C32" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" s="46">
         <v>43361</v>
@@ -3366,7 +3386,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D36" s="46">
         <v>43360</v>
@@ -3480,7 +3500,7 @@
         <v>37</v>
       </c>
       <c r="C40" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D40" s="46">
         <v>43360</v>
@@ -3594,7 +3614,7 @@
         <v>37</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D44" s="46">
         <v>43360</v>
@@ -3708,7 +3728,7 @@
         <v>37</v>
       </c>
       <c r="C48" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D48" s="46">
         <v>43360</v>
@@ -3854,7 +3874,7 @@
         <v>37</v>
       </c>
       <c r="C53" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D53" s="83">
         <v>43360</v>
@@ -4000,7 +4020,7 @@
         <v>37</v>
       </c>
       <c r="C58" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D58" s="83">
         <v>43361</v>
@@ -4114,7 +4134,7 @@
         <v>37</v>
       </c>
       <c r="C62" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D62" s="46">
         <v>43362</v>
@@ -4228,7 +4248,7 @@
         <v>37</v>
       </c>
       <c r="C66" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D66" s="46">
         <v>43360</v>
@@ -4342,7 +4362,7 @@
         <v>37</v>
       </c>
       <c r="C70" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D70" s="46">
         <v>43363</v>
@@ -4456,7 +4476,7 @@
         <v>37</v>
       </c>
       <c r="C74" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D74" s="46">
         <v>43355</v>
@@ -4986,7 +5006,7 @@
         <v>37</v>
       </c>
       <c r="C91" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D91" s="46">
         <v>43355</v>
@@ -5228,7 +5248,7 @@
         <v>37</v>
       </c>
       <c r="C99" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D99" s="46">
         <v>43312</v>
@@ -5240,7 +5260,7 @@
         <v>31</v>
       </c>
       <c r="G99" s="48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I99" s="53"/>
       <c r="J99" s="54"/>
@@ -5260,7 +5280,7 @@
         <v>37</v>
       </c>
       <c r="C100" s="47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D100" s="46">
         <v>43319</v>
@@ -5292,7 +5312,7 @@
         <v>37</v>
       </c>
       <c r="C101" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D101" s="46">
         <v>43360</v>
@@ -5470,7 +5490,7 @@
         <v>37</v>
       </c>
       <c r="C107" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D107" s="46">
         <v>43360</v>
@@ -5840,7 +5860,7 @@
         <v>37</v>
       </c>
       <c r="C119" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D119" s="46">
         <v>43361</v>
@@ -6018,7 +6038,7 @@
         <v>37</v>
       </c>
       <c r="C125" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D125" s="46">
         <v>43360</v>
@@ -6196,7 +6216,7 @@
         <v>37</v>
       </c>
       <c r="C131" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D131" s="46">
         <v>43356</v>
@@ -6510,7 +6530,7 @@
         <v>37</v>
       </c>
       <c r="C141" s="47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D141" s="46">
         <v>43277</v>
@@ -6522,7 +6542,7 @@
         <v>31</v>
       </c>
       <c r="G141" s="87" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H141" s="1"/>
       <c r="I141" s="53"/>
@@ -6543,7 +6563,7 @@
         <v>37</v>
       </c>
       <c r="C142" s="47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D142" s="46">
         <v>43290</v>
@@ -6576,7 +6596,7 @@
         <v>37</v>
       </c>
       <c r="C143" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D143" s="46">
         <v>43313</v>
@@ -6588,7 +6608,7 @@
         <v>31</v>
       </c>
       <c r="G143" s="87" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H143" s="1"/>
       <c r="I143" s="53"/>
@@ -6609,7 +6629,7 @@
         <v>37</v>
       </c>
       <c r="C144" s="47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D144" s="46">
         <v>43319</v>
@@ -6642,7 +6662,7 @@
         <v>37</v>
       </c>
       <c r="C145" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D145" s="46">
         <v>43363</v>
@@ -6793,7 +6813,7 @@
         <v>37</v>
       </c>
       <c r="C150" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D150" s="46">
         <v>43360</v>
@@ -6911,7 +6931,7 @@
         <v>37</v>
       </c>
       <c r="C154" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D154" s="46">
         <v>43354</v>
@@ -7029,7 +7049,7 @@
         <v>37</v>
       </c>
       <c r="C158" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D158" s="46">
         <v>43354</v>
@@ -7180,7 +7200,7 @@
         <v>37</v>
       </c>
       <c r="C163" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D163" s="46">
         <v>43356</v>
@@ -7364,7 +7384,7 @@
         <v>37</v>
       </c>
       <c r="C169" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D169" s="46">
         <v>43354</v>
@@ -7410,7 +7430,7 @@
     </row>
     <row r="171" spans="1:17" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A171" s="47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B171" s="48" t="s">
         <v>37</v>
@@ -7443,13 +7463,13 @@
     </row>
     <row r="172" spans="1:17" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A172" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B172" s="48" t="s">
         <v>37</v>
       </c>
       <c r="C172" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D172" s="46">
         <v>43354</v>
@@ -7567,7 +7587,7 @@
         <v>37</v>
       </c>
       <c r="C176" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D176" s="46">
         <v>43355</v>
@@ -7685,7 +7705,7 @@
         <v>37</v>
       </c>
       <c r="C180" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D180" s="46">
         <v>43355</v>
@@ -7803,7 +7823,7 @@
         <v>37</v>
       </c>
       <c r="C184" s="49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D184" s="46">
         <v>43291</v>
@@ -7815,7 +7835,7 @@
         <v>31</v>
       </c>
       <c r="G184" s="48" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H184" s="1"/>
       <c r="I184" s="22"/>
@@ -7836,7 +7856,7 @@
         <v>37</v>
       </c>
       <c r="C185" s="49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D185" s="46">
         <v>43298</v>
@@ -7869,7 +7889,7 @@
         <v>37</v>
       </c>
       <c r="C186" s="88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D186" s="83">
         <v>43356</v>
@@ -7987,7 +8007,7 @@
         <v>37</v>
       </c>
       <c r="C190" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D190" s="46">
         <v>43356</v>
@@ -8105,7 +8125,7 @@
         <v>37</v>
       </c>
       <c r="C194" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D194" s="46">
         <v>43356</v>
@@ -8223,7 +8243,7 @@
         <v>37</v>
       </c>
       <c r="C198" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D198" s="46">
         <v>43355</v>
@@ -8407,7 +8427,7 @@
         <v>37</v>
       </c>
       <c r="C204" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D204" s="68">
         <v>43355</v>
@@ -8525,7 +8545,7 @@
         <v>37</v>
       </c>
       <c r="C208" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D208" s="68">
         <v>43355</v>
@@ -8604,13 +8624,13 @@
     </row>
     <row r="211" spans="1:17" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A211" s="47" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B211" s="48" t="s">
         <v>37</v>
       </c>
       <c r="C211" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D211" s="46">
         <v>43355</v>
@@ -8695,7 +8715,7 @@
         <v>37</v>
       </c>
       <c r="C214" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D214" s="46">
         <v>43354</v>
@@ -8739,14 +8759,28 @@
       <c r="P215" s="22"/>
       <c r="Q215" s="22"/>
     </row>
-    <row r="216" spans="1:17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="78"/>
-      <c r="B216" s="67"/>
-      <c r="C216" s="67"/>
-      <c r="D216" s="46"/>
-      <c r="E216" s="47"/>
-      <c r="F216" s="67"/>
-      <c r="G216" s="48"/>
+    <row r="216" spans="1:17" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A216" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="B216" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="C216" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="D216" s="46">
+        <v>43157</v>
+      </c>
+      <c r="E216" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F216" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="G216" s="48" t="s">
+        <v>15</v>
+      </c>
       <c r="H216" s="1"/>
       <c r="I216" s="22"/>
       <c r="J216" s="22"/>
@@ -8758,14 +8792,28 @@
       <c r="P216" s="22"/>
       <c r="Q216" s="22"/>
     </row>
-    <row r="217" spans="1:17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="47"/>
-      <c r="B217" s="67"/>
-      <c r="C217" s="67"/>
-      <c r="D217" s="46"/>
-      <c r="E217" s="47"/>
-      <c r="F217" s="67"/>
-      <c r="G217" s="48"/>
+    <row r="217" spans="1:17" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="B217" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C217" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D217" s="46">
+        <v>43354</v>
+      </c>
+      <c r="E217" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="F217" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G217" s="48" t="s">
+        <v>15</v>
+      </c>
       <c r="H217" s="1"/>
       <c r="I217" s="22"/>
       <c r="J217" s="22"/>

</xml_diff>